<commit_message>
Refactor examples, add CLI, add validation tests
</commit_message>
<xml_diff>
--- a/examples/neutralization-submission-invalid-highlighted.xlsx
+++ b/examples/neutralization-submission-invalid-highlighted.xlsx
@@ -75,6 +75,11 @@
     <author>Validation service</author>
   </authors>
   <commentList>
+    <comment authorId="0" ref="A3" shapeId="0">
+      <text>
+        <t>Missing required value for 'Antibody name'</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="A4" shapeId="0">
       <text>
         <t>Duplicate value 'COVIC 1' is not allowed for 'Antibody name'</t>
@@ -87,7 +92,7 @@
     </comment>
     <comment authorId="0" ref="C6" shapeId="0">
       <text>
-        <t>'none' is not of type 'float'</t>
+        <t>'none' is not of type 'float' in 'Titer'</t>
       </text>
     </comment>
     <comment authorId="0" ref="B7" shapeId="0">
@@ -505,7 +510,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
+      <c r="A3" s="2" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
           <t>negative</t>

</xml_diff>